<commit_message>
OUCD and XLSX Time Spent per UC updated
</commit_message>
<xml_diff>
--- a/UseCases/TimeSpentPerUC.xlsx
+++ b/UseCases/TimeSpentPerUC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wzielke\Desktop\Software Engineering\FitnessWebAppDocumentation\FitnessWebAppDocumentation\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1CEC7B-FAC6-49ED-8398-D4C7F68EE90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E5775C-C1B4-4E8F-915B-97847E1E8C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>UC</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Calculated Time (min)</t>
+  </si>
+  <si>
+    <t>Time Spent for calc. Ucs</t>
   </si>
 </sst>
 </file>
@@ -133,9 +136,8 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -259,11 +261,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -319,15 +382,39 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,10 +721,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,221 +1047,215 @@
       </c>
       <c r="H16" s="18"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="21" t="s">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="C47" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="D47" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="E47" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="26"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="23" t="s">
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="27">
+      <c r="C48" s="25">
         <v>376.2</v>
       </c>
-      <c r="C48" s="19">
-        <v>937</v>
-      </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="26"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="23" t="s">
+      <c r="D48" s="19">
+        <v>1153</v>
+      </c>
+      <c r="E48" s="19"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="27">
+      <c r="C49" s="25">
         <v>144.44999999999999</v>
       </c>
-      <c r="C49" s="19">
-        <v>737</v>
-      </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="26"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="23" t="s">
+      <c r="D49" s="19">
+        <v>953</v>
+      </c>
+      <c r="E49" s="19"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="27">
+      <c r="C50" s="25">
         <v>134.82</v>
       </c>
-      <c r="C50" s="19">
-        <v>725</v>
-      </c>
-      <c r="D50" s="19"/>
-      <c r="E50" s="26"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="23" t="s">
+      <c r="D50" s="19">
+        <v>941</v>
+      </c>
+      <c r="E50" s="19"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="27">
+      <c r="C51" s="25">
         <v>108.07</v>
       </c>
-      <c r="C51" s="19">
-        <v>485</v>
-      </c>
-      <c r="D51" s="19"/>
-      <c r="E51" s="26"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="23" t="s">
+      <c r="D51" s="19">
+        <v>701</v>
+      </c>
+      <c r="E51" s="19"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="27">
+      <c r="C52" s="25">
         <v>166.92</v>
       </c>
-      <c r="C52" s="19">
-        <v>485</v>
-      </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="26"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="23" t="s">
+      <c r="D52" s="19">
+        <v>701</v>
+      </c>
+      <c r="E52" s="19"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="27">
+      <c r="C53" s="25">
         <v>41</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="20">
+      <c r="D53" s="33">
+        <v>1140</v>
+      </c>
+      <c r="E53" s="20">
         <v>551</v>
       </c>
-      <c r="E53" s="26"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="23" t="s">
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="27">
+      <c r="C54" s="25">
         <v>37</v>
       </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="20">
+      <c r="D54" s="34"/>
+      <c r="E54" s="20">
         <v>542</v>
       </c>
-      <c r="E54" s="26"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="23" t="s">
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="27">
+      <c r="C55" s="25">
         <v>31</v>
       </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="20">
+      <c r="D55" s="35"/>
+      <c r="E55" s="20">
         <v>528</v>
       </c>
-      <c r="E55" s="26"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="23" t="s">
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="27">
+      <c r="C56" s="25">
         <v>44</v>
       </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="20">
+      <c r="D56" s="33">
+        <v>1140</v>
+      </c>
+      <c r="E56" s="20">
         <v>558</v>
       </c>
-      <c r="E56" s="26"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="23" t="s">
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="27">
+      <c r="C57" s="25">
         <v>35</v>
       </c>
-      <c r="C57" s="19"/>
-      <c r="D57" s="20">
+      <c r="D57" s="35"/>
+      <c r="E57" s="20">
         <v>537</v>
       </c>
-      <c r="E57" s="26"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="23" t="s">
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B58" s="27">
+      <c r="C58" s="25">
         <v>373</v>
       </c>
-      <c r="C58" s="19"/>
-      <c r="D58" s="20">
+      <c r="D58" s="36">
+        <v>1440</v>
+      </c>
+      <c r="E58" s="20">
         <v>1326</v>
       </c>
-      <c r="E58" s="26"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="23" t="s">
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="27">
+      <c r="C59" s="25">
         <v>22</v>
       </c>
-      <c r="C59" s="19"/>
-      <c r="D59" s="20">
+      <c r="D59" s="37"/>
+      <c r="E59" s="20">
         <v>507</v>
       </c>
-      <c r="E59" s="26"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="23" t="s">
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="27">
+      <c r="C60" s="25">
         <v>26</v>
       </c>
-      <c r="C60" s="19"/>
-      <c r="D60" s="20">
+      <c r="D60" s="38"/>
+      <c r="E60" s="20">
         <v>516</v>
       </c>
-      <c r="E60" s="26"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" s="27"/>
-      <c r="C61" s="19">
-        <v>1080</v>
-      </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="26"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62" s="28">
-        <f>SUM(B48:B61)</f>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="25">
+        <v>166.92</v>
+      </c>
+      <c r="D61" s="27">
+        <f>SUM(D53+D56+D58)</f>
+        <v>3720</v>
+      </c>
+      <c r="E61" s="31">
+        <f>SUM(E48:E60)</f>
+        <v>5065</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="26">
+        <f ca="1">SUM(C48:C62)</f>
         <v>1539.46</v>
       </c>
-      <c r="C62" s="25">
-        <f>SUM(C48:C61)</f>
-        <v>4449</v>
-      </c>
-      <c r="D62" s="25">
-        <f>SUM(D48:D61)</f>
-        <v>5065</v>
-      </c>
-      <c r="E62" s="25">
-        <f>SUM(C62,D62)</f>
-        <v>9514</v>
-      </c>
+      <c r="D62" s="29">
+        <f>SUM(D48:D60)</f>
+        <v>8169</v>
+      </c>
+      <c r="E62" s="32"/>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D65" s="28"/>
+      <c r="E65" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>